<commit_message>
WORK IN PROGRESS: Updating the TV input data, and preparing to add a miscellaneous baseload.
</commit_message>
<xml_diff>
--- a/bcd/CREST/ValidationSet.xlsx
+++ b/bcd/CREST/ValidationSet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>Record</t>
   </si>
@@ -271,6 +271,33 @@
   </si>
   <si>
     <t>non-HVAC [GJ]</t>
+  </si>
+  <si>
+    <t>H01</t>
+  </si>
+  <si>
+    <t>H02</t>
+  </si>
+  <si>
+    <t>H03</t>
+  </si>
+  <si>
+    <t>H04</t>
+  </si>
+  <si>
+    <t>H05</t>
+  </si>
+  <si>
+    <t>H06</t>
+  </si>
+  <si>
+    <t>H07</t>
+  </si>
+  <si>
+    <t>H09</t>
+  </si>
+  <si>
+    <t>non-HVAC [kWh]</t>
   </si>
 </sst>
 </file>
@@ -788,14 +815,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -821,6 +842,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1163,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:QQ28"/>
+  <dimension ref="A1:QQ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,42 +1206,42 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="25"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:459" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:459" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:459" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1224,7 +1256,7 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
@@ -1239,7 +1271,7 @@
       <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1288,462 +1320,462 @@
       <c r="E5">
         <v>18.2</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>1953</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>165.54</v>
       </c>
       <c r="J5">
         <v>4</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="5"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="5"/>
-      <c r="AO5" s="5"/>
-      <c r="AP5" s="5"/>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="5"/>
-      <c r="AT5" s="5"/>
-      <c r="AU5" s="5"/>
-      <c r="AV5" s="5"/>
-      <c r="AW5" s="5"/>
-      <c r="AX5" s="5"/>
-      <c r="AY5" s="5"/>
-      <c r="AZ5" s="5"/>
-      <c r="BA5" s="5"/>
-      <c r="BB5" s="5"/>
-      <c r="BC5" s="5"/>
-      <c r="BD5" s="5"/>
-      <c r="BE5" s="5"/>
-      <c r="BF5" s="5"/>
-      <c r="BG5" s="5"/>
-      <c r="BH5" s="5"/>
-      <c r="BI5" s="5"/>
-      <c r="BJ5" s="5"/>
-      <c r="BK5" s="5"/>
-      <c r="BL5" s="5"/>
-      <c r="BM5" s="5"/>
-      <c r="BN5" s="5"/>
-      <c r="BO5" s="5"/>
-      <c r="BP5" s="5"/>
-      <c r="BQ5" s="5"/>
-      <c r="BR5" s="5"/>
-      <c r="BS5" s="5"/>
-      <c r="BT5" s="5"/>
-      <c r="BU5" s="5"/>
-      <c r="BV5" s="5"/>
-      <c r="BW5" s="5"/>
-      <c r="BX5" s="5"/>
-      <c r="BY5" s="5"/>
-      <c r="BZ5" s="5"/>
-      <c r="CA5" s="5"/>
-      <c r="CB5" s="5"/>
-      <c r="CC5" s="5"/>
-      <c r="CD5" s="5"/>
-      <c r="CE5" s="5"/>
-      <c r="CF5" s="5"/>
-      <c r="CG5" s="5"/>
-      <c r="CH5" s="5"/>
-      <c r="CI5" s="5"/>
-      <c r="CJ5" s="5"/>
-      <c r="CK5" s="5"/>
-      <c r="CL5" s="5"/>
-      <c r="CM5" s="5"/>
-      <c r="CN5" s="5"/>
-      <c r="CO5" s="5"/>
-      <c r="CP5" s="5"/>
-      <c r="CQ5" s="5"/>
-      <c r="CR5" s="5"/>
-      <c r="CS5" s="5"/>
-      <c r="CT5" s="5"/>
-      <c r="CU5" s="5"/>
-      <c r="CV5" s="5"/>
-      <c r="CW5" s="5"/>
-      <c r="CX5" s="5"/>
-      <c r="CY5" s="5"/>
-      <c r="CZ5" s="5"/>
-      <c r="DA5" s="5"/>
-      <c r="DB5" s="5"/>
-      <c r="DC5" s="5"/>
-      <c r="DD5" s="5"/>
-      <c r="DE5" s="5"/>
-      <c r="DF5" s="5"/>
-      <c r="DG5" s="5"/>
-      <c r="DH5" s="5"/>
-      <c r="DI5" s="5"/>
-      <c r="DJ5" s="5"/>
-      <c r="DK5" s="5"/>
-      <c r="DL5" s="5"/>
-      <c r="DM5" s="5"/>
-      <c r="DN5" s="5"/>
-      <c r="DO5" s="5"/>
-      <c r="DP5" s="5"/>
-      <c r="DQ5" s="5"/>
-      <c r="DR5" s="5"/>
-      <c r="DS5" s="5"/>
-      <c r="DT5" s="5"/>
-      <c r="DU5" s="5"/>
-      <c r="DV5" s="5"/>
-      <c r="DW5" s="5"/>
-      <c r="DX5" s="5"/>
-      <c r="DY5" s="5"/>
-      <c r="DZ5" s="5"/>
-      <c r="EA5" s="5"/>
-      <c r="EB5" s="5"/>
-      <c r="EC5" s="5"/>
-      <c r="ED5" s="5"/>
-      <c r="EE5" s="5"/>
-      <c r="EF5" s="5"/>
-      <c r="EG5" s="5"/>
-      <c r="EH5" s="5"/>
-      <c r="EI5" s="5"/>
-      <c r="EJ5" s="5"/>
-      <c r="EK5" s="5"/>
-      <c r="EL5" s="5"/>
-      <c r="EM5" s="5"/>
-      <c r="EN5" s="5"/>
-      <c r="EO5" s="5"/>
-      <c r="EP5" s="5"/>
-      <c r="EQ5" s="5"/>
-      <c r="ER5" s="5"/>
-      <c r="ES5" s="5"/>
-      <c r="ET5" s="5"/>
-      <c r="EU5" s="5"/>
-      <c r="EV5" s="5"/>
-      <c r="EW5" s="5"/>
-      <c r="EX5" s="5"/>
-      <c r="EY5" s="5"/>
-      <c r="EZ5" s="5"/>
-      <c r="FA5" s="5"/>
-      <c r="FB5" s="5"/>
-      <c r="FC5" s="5"/>
-      <c r="FD5" s="5"/>
-      <c r="FE5" s="5"/>
-      <c r="FF5" s="5"/>
-      <c r="FG5" s="5"/>
-      <c r="FH5" s="5"/>
-      <c r="FI5" s="5"/>
-      <c r="FJ5" s="5"/>
-      <c r="FK5" s="5"/>
-      <c r="FL5" s="5"/>
-      <c r="FM5" s="5"/>
-      <c r="FN5" s="5"/>
-      <c r="FO5" s="5"/>
-      <c r="FP5" s="5"/>
-      <c r="FQ5" s="5"/>
-      <c r="FR5" s="5"/>
-      <c r="FS5" s="5"/>
-      <c r="FT5" s="5"/>
-      <c r="FU5" s="5"/>
-      <c r="FV5" s="5"/>
-      <c r="FW5" s="5"/>
-      <c r="FX5" s="5"/>
-      <c r="FY5" s="5"/>
-      <c r="FZ5" s="5"/>
-      <c r="GA5" s="5"/>
-      <c r="GB5" s="5"/>
-      <c r="GC5" s="5"/>
-      <c r="GD5" s="5"/>
-      <c r="GE5" s="5"/>
-      <c r="GF5" s="5"/>
-      <c r="GG5" s="5"/>
-      <c r="GH5" s="5"/>
-      <c r="GI5" s="5"/>
-      <c r="GJ5" s="5"/>
-      <c r="GK5" s="5"/>
-      <c r="GL5" s="5"/>
-      <c r="GM5" s="5"/>
-      <c r="GN5" s="5"/>
-      <c r="GO5" s="5"/>
-      <c r="GP5" s="5"/>
-      <c r="GQ5" s="5"/>
-      <c r="GR5" s="5"/>
-      <c r="GS5" s="5"/>
-      <c r="GT5" s="5"/>
-      <c r="GU5" s="5"/>
-      <c r="GV5" s="5"/>
-      <c r="GW5" s="5"/>
-      <c r="GX5" s="5"/>
-      <c r="GY5" s="5"/>
-      <c r="GZ5" s="5"/>
-      <c r="HA5" s="5"/>
-      <c r="HB5" s="5"/>
-      <c r="HC5" s="5"/>
-      <c r="HD5" s="5"/>
-      <c r="HE5" s="5"/>
-      <c r="HF5" s="5"/>
-      <c r="HG5" s="5"/>
-      <c r="HH5" s="5"/>
-      <c r="HI5" s="5"/>
-      <c r="HJ5" s="5"/>
-      <c r="HK5" s="5"/>
-      <c r="HL5" s="5"/>
-      <c r="HM5" s="5"/>
-      <c r="HN5" s="5"/>
-      <c r="HO5" s="5"/>
-      <c r="HP5" s="5"/>
-      <c r="HQ5" s="5"/>
-      <c r="HR5" s="5"/>
-      <c r="HS5" s="5"/>
-      <c r="HT5" s="5"/>
-      <c r="HU5" s="5"/>
-      <c r="HV5" s="5"/>
-      <c r="HW5" s="5"/>
-      <c r="HX5" s="5"/>
-      <c r="HY5" s="5"/>
-      <c r="HZ5" s="5"/>
-      <c r="IA5" s="5"/>
-      <c r="IB5" s="5"/>
-      <c r="IC5" s="5"/>
-      <c r="ID5" s="5"/>
-      <c r="IE5" s="5"/>
-      <c r="IF5" s="5"/>
-      <c r="IG5" s="5"/>
-      <c r="IH5" s="5"/>
-      <c r="II5" s="5"/>
-      <c r="IJ5" s="5"/>
-      <c r="IK5" s="5"/>
-      <c r="IL5" s="5"/>
-      <c r="IM5" s="5"/>
-      <c r="IN5" s="5"/>
-      <c r="IO5" s="5"/>
-      <c r="IP5" s="5"/>
-      <c r="IQ5" s="5"/>
-      <c r="IR5" s="5"/>
-      <c r="IS5" s="5"/>
-      <c r="IT5" s="5"/>
-      <c r="IU5" s="5"/>
-      <c r="IV5" s="5"/>
-      <c r="IW5" s="5"/>
-      <c r="IX5" s="5"/>
-      <c r="IY5" s="5"/>
-      <c r="IZ5" s="5"/>
-      <c r="JA5" s="5"/>
-      <c r="JB5" s="5"/>
-      <c r="JC5" s="5"/>
-      <c r="JD5" s="5"/>
-      <c r="JE5" s="5"/>
-      <c r="JF5" s="5"/>
-      <c r="JG5" s="5"/>
-      <c r="JH5" s="5"/>
-      <c r="JI5" s="5"/>
-      <c r="JJ5" s="5"/>
-      <c r="JK5" s="5"/>
-      <c r="JL5" s="5"/>
-      <c r="JM5" s="5"/>
-      <c r="JN5" s="5"/>
-      <c r="JO5" s="5"/>
-      <c r="JP5" s="5"/>
-      <c r="JQ5" s="5"/>
-      <c r="JR5" s="5"/>
-      <c r="JS5" s="5"/>
-      <c r="JT5" s="5"/>
-      <c r="JU5" s="5"/>
-      <c r="JV5" s="5"/>
-      <c r="JW5" s="5"/>
-      <c r="JX5" s="5"/>
-      <c r="JY5" s="5"/>
-      <c r="JZ5" s="5"/>
-      <c r="KA5" s="5"/>
-      <c r="KB5" s="5"/>
-      <c r="KC5" s="5"/>
-      <c r="KD5" s="5"/>
-      <c r="KE5" s="5"/>
-      <c r="KF5" s="5"/>
-      <c r="KG5" s="5"/>
-      <c r="KH5" s="5"/>
-      <c r="KI5" s="5"/>
-      <c r="KJ5" s="5"/>
-      <c r="KK5" s="5"/>
-      <c r="KL5" s="5"/>
-      <c r="KM5" s="5"/>
-      <c r="KN5" s="5"/>
-      <c r="KO5" s="5"/>
-      <c r="KP5" s="5"/>
-      <c r="KQ5" s="5"/>
-      <c r="KR5" s="5"/>
-      <c r="KS5" s="5"/>
-      <c r="KT5" s="5"/>
-      <c r="KU5" s="5"/>
-      <c r="KV5" s="5"/>
-      <c r="KW5" s="5"/>
-      <c r="KX5" s="5"/>
-      <c r="KY5" s="5"/>
-      <c r="KZ5" s="5"/>
-      <c r="LA5" s="5"/>
-      <c r="LB5" s="5"/>
-      <c r="LC5" s="5"/>
-      <c r="LD5" s="5"/>
-      <c r="LE5" s="5"/>
-      <c r="LF5" s="5"/>
-      <c r="LG5" s="5"/>
-      <c r="LH5" s="5"/>
-      <c r="LI5" s="5"/>
-      <c r="LJ5" s="5"/>
-      <c r="LK5" s="5"/>
-      <c r="LL5" s="5"/>
-      <c r="LM5" s="5"/>
-      <c r="LN5" s="5"/>
-      <c r="LO5" s="5"/>
-      <c r="LP5" s="5"/>
-      <c r="LQ5" s="5"/>
-      <c r="LR5" s="5"/>
-      <c r="LS5" s="5"/>
-      <c r="LT5" s="5"/>
-      <c r="LU5" s="5"/>
-      <c r="LV5" s="5"/>
-      <c r="LW5" s="5"/>
-      <c r="LX5" s="5"/>
-      <c r="LY5" s="5"/>
-      <c r="LZ5" s="5"/>
-      <c r="MA5" s="5"/>
-      <c r="MB5" s="5"/>
-      <c r="MC5" s="5"/>
-      <c r="MD5" s="5"/>
-      <c r="ME5" s="5"/>
-      <c r="MF5" s="5"/>
-      <c r="MG5" s="5"/>
-      <c r="MH5" s="5"/>
-      <c r="MI5" s="5"/>
-      <c r="MJ5" s="5"/>
-      <c r="MK5" s="5"/>
-      <c r="ML5" s="5"/>
-      <c r="MM5" s="5"/>
-      <c r="MN5" s="5"/>
-      <c r="MO5" s="5"/>
-      <c r="MP5" s="5"/>
-      <c r="MQ5" s="5"/>
-      <c r="MR5" s="5"/>
-      <c r="MS5" s="5"/>
-      <c r="MT5" s="5"/>
-      <c r="MU5" s="5"/>
-      <c r="MV5" s="5"/>
-      <c r="MW5" s="5"/>
-      <c r="MX5" s="5"/>
-      <c r="MY5" s="5"/>
-      <c r="MZ5" s="5"/>
-      <c r="NA5" s="5"/>
-      <c r="NB5" s="5"/>
-      <c r="NC5" s="5"/>
-      <c r="ND5" s="5"/>
-      <c r="NE5" s="5"/>
-      <c r="NF5" s="5"/>
-      <c r="NG5" s="5"/>
-      <c r="NH5" s="5"/>
-      <c r="NI5" s="5"/>
-      <c r="NJ5" s="5"/>
-      <c r="NK5" s="5"/>
-      <c r="NL5" s="5"/>
-      <c r="NM5" s="5"/>
-      <c r="NN5" s="5"/>
-      <c r="NO5" s="5"/>
-      <c r="NP5" s="5"/>
-      <c r="NQ5" s="5"/>
-      <c r="NR5" s="5"/>
-      <c r="NS5" s="5"/>
-      <c r="NT5" s="5"/>
-      <c r="NU5" s="5"/>
-      <c r="NV5" s="5"/>
-      <c r="NW5" s="5"/>
-      <c r="NX5" s="5"/>
-      <c r="NY5" s="5"/>
-      <c r="NZ5" s="5"/>
-      <c r="OA5" s="5"/>
-      <c r="OB5" s="5"/>
-      <c r="OC5" s="5"/>
-      <c r="OD5" s="5"/>
-      <c r="OE5" s="5"/>
-      <c r="OF5" s="5"/>
-      <c r="OG5" s="5"/>
-      <c r="OH5" s="5"/>
-      <c r="OI5" s="5"/>
-      <c r="OJ5" s="5"/>
-      <c r="OK5" s="5"/>
-      <c r="OL5" s="5"/>
-      <c r="OM5" s="5"/>
-      <c r="ON5" s="5"/>
-      <c r="OO5" s="5"/>
-      <c r="OP5" s="5"/>
-      <c r="OQ5" s="5"/>
-      <c r="OR5" s="5"/>
-      <c r="OS5" s="5"/>
-      <c r="OT5" s="5"/>
-      <c r="OU5" s="5"/>
-      <c r="OV5" s="5"/>
-      <c r="OW5" s="5"/>
-      <c r="OX5" s="5"/>
-      <c r="OY5" s="5"/>
-      <c r="OZ5" s="5"/>
-      <c r="PA5" s="5"/>
-      <c r="PB5" s="5"/>
-      <c r="PC5" s="5"/>
-      <c r="PD5" s="5"/>
-      <c r="PE5" s="5"/>
-      <c r="PF5" s="5"/>
-      <c r="PG5" s="5"/>
-      <c r="PH5" s="5"/>
-      <c r="PI5" s="5"/>
-      <c r="PJ5" s="5"/>
-      <c r="PK5" s="5"/>
-      <c r="PL5" s="5"/>
-      <c r="PM5" s="5"/>
-      <c r="PN5" s="5"/>
-      <c r="PO5" s="5"/>
-      <c r="PP5" s="5"/>
-      <c r="PQ5" s="5"/>
-      <c r="PR5" s="5"/>
-      <c r="PS5" s="5"/>
-      <c r="PT5" s="5"/>
-      <c r="PU5" s="5"/>
-      <c r="PV5" s="5"/>
-      <c r="PW5" s="5"/>
-      <c r="PX5" s="5"/>
-      <c r="PY5" s="5"/>
-      <c r="PZ5" s="5"/>
-      <c r="QA5" s="5"/>
-      <c r="QB5" s="5"/>
-      <c r="QC5" s="5"/>
-      <c r="QD5" s="5"/>
-      <c r="QE5" s="5"/>
-      <c r="QF5" s="5"/>
-      <c r="QG5" s="5"/>
-      <c r="QH5" s="5"/>
-      <c r="QI5" s="5"/>
-      <c r="QJ5" s="5"/>
-      <c r="QK5" s="5"/>
-      <c r="QL5" s="5"/>
-      <c r="QM5" s="5"/>
-      <c r="QN5" s="5"/>
-      <c r="QO5" s="5"/>
-      <c r="QP5" s="5"/>
-      <c r="QQ5" s="5"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="3"/>
+      <c r="AV5" s="3"/>
+      <c r="AW5" s="3"/>
+      <c r="AX5" s="3"/>
+      <c r="AY5" s="3"/>
+      <c r="AZ5" s="3"/>
+      <c r="BA5" s="3"/>
+      <c r="BB5" s="3"/>
+      <c r="BC5" s="3"/>
+      <c r="BD5" s="3"/>
+      <c r="BE5" s="3"/>
+      <c r="BF5" s="3"/>
+      <c r="BG5" s="3"/>
+      <c r="BH5" s="3"/>
+      <c r="BI5" s="3"/>
+      <c r="BJ5" s="3"/>
+      <c r="BK5" s="3"/>
+      <c r="BL5" s="3"/>
+      <c r="BM5" s="3"/>
+      <c r="BN5" s="3"/>
+      <c r="BO5" s="3"/>
+      <c r="BP5" s="3"/>
+      <c r="BQ5" s="3"/>
+      <c r="BR5" s="3"/>
+      <c r="BS5" s="3"/>
+      <c r="BT5" s="3"/>
+      <c r="BU5" s="3"/>
+      <c r="BV5" s="3"/>
+      <c r="BW5" s="3"/>
+      <c r="BX5" s="3"/>
+      <c r="BY5" s="3"/>
+      <c r="BZ5" s="3"/>
+      <c r="CA5" s="3"/>
+      <c r="CB5" s="3"/>
+      <c r="CC5" s="3"/>
+      <c r="CD5" s="3"/>
+      <c r="CE5" s="3"/>
+      <c r="CF5" s="3"/>
+      <c r="CG5" s="3"/>
+      <c r="CH5" s="3"/>
+      <c r="CI5" s="3"/>
+      <c r="CJ5" s="3"/>
+      <c r="CK5" s="3"/>
+      <c r="CL5" s="3"/>
+      <c r="CM5" s="3"/>
+      <c r="CN5" s="3"/>
+      <c r="CO5" s="3"/>
+      <c r="CP5" s="3"/>
+      <c r="CQ5" s="3"/>
+      <c r="CR5" s="3"/>
+      <c r="CS5" s="3"/>
+      <c r="CT5" s="3"/>
+      <c r="CU5" s="3"/>
+      <c r="CV5" s="3"/>
+      <c r="CW5" s="3"/>
+      <c r="CX5" s="3"/>
+      <c r="CY5" s="3"/>
+      <c r="CZ5" s="3"/>
+      <c r="DA5" s="3"/>
+      <c r="DB5" s="3"/>
+      <c r="DC5" s="3"/>
+      <c r="DD5" s="3"/>
+      <c r="DE5" s="3"/>
+      <c r="DF5" s="3"/>
+      <c r="DG5" s="3"/>
+      <c r="DH5" s="3"/>
+      <c r="DI5" s="3"/>
+      <c r="DJ5" s="3"/>
+      <c r="DK5" s="3"/>
+      <c r="DL5" s="3"/>
+      <c r="DM5" s="3"/>
+      <c r="DN5" s="3"/>
+      <c r="DO5" s="3"/>
+      <c r="DP5" s="3"/>
+      <c r="DQ5" s="3"/>
+      <c r="DR5" s="3"/>
+      <c r="DS5" s="3"/>
+      <c r="DT5" s="3"/>
+      <c r="DU5" s="3"/>
+      <c r="DV5" s="3"/>
+      <c r="DW5" s="3"/>
+      <c r="DX5" s="3"/>
+      <c r="DY5" s="3"/>
+      <c r="DZ5" s="3"/>
+      <c r="EA5" s="3"/>
+      <c r="EB5" s="3"/>
+      <c r="EC5" s="3"/>
+      <c r="ED5" s="3"/>
+      <c r="EE5" s="3"/>
+      <c r="EF5" s="3"/>
+      <c r="EG5" s="3"/>
+      <c r="EH5" s="3"/>
+      <c r="EI5" s="3"/>
+      <c r="EJ5" s="3"/>
+      <c r="EK5" s="3"/>
+      <c r="EL5" s="3"/>
+      <c r="EM5" s="3"/>
+      <c r="EN5" s="3"/>
+      <c r="EO5" s="3"/>
+      <c r="EP5" s="3"/>
+      <c r="EQ5" s="3"/>
+      <c r="ER5" s="3"/>
+      <c r="ES5" s="3"/>
+      <c r="ET5" s="3"/>
+      <c r="EU5" s="3"/>
+      <c r="EV5" s="3"/>
+      <c r="EW5" s="3"/>
+      <c r="EX5" s="3"/>
+      <c r="EY5" s="3"/>
+      <c r="EZ5" s="3"/>
+      <c r="FA5" s="3"/>
+      <c r="FB5" s="3"/>
+      <c r="FC5" s="3"/>
+      <c r="FD5" s="3"/>
+      <c r="FE5" s="3"/>
+      <c r="FF5" s="3"/>
+      <c r="FG5" s="3"/>
+      <c r="FH5" s="3"/>
+      <c r="FI5" s="3"/>
+      <c r="FJ5" s="3"/>
+      <c r="FK5" s="3"/>
+      <c r="FL5" s="3"/>
+      <c r="FM5" s="3"/>
+      <c r="FN5" s="3"/>
+      <c r="FO5" s="3"/>
+      <c r="FP5" s="3"/>
+      <c r="FQ5" s="3"/>
+      <c r="FR5" s="3"/>
+      <c r="FS5" s="3"/>
+      <c r="FT5" s="3"/>
+      <c r="FU5" s="3"/>
+      <c r="FV5" s="3"/>
+      <c r="FW5" s="3"/>
+      <c r="FX5" s="3"/>
+      <c r="FY5" s="3"/>
+      <c r="FZ5" s="3"/>
+      <c r="GA5" s="3"/>
+      <c r="GB5" s="3"/>
+      <c r="GC5" s="3"/>
+      <c r="GD5" s="3"/>
+      <c r="GE5" s="3"/>
+      <c r="GF5" s="3"/>
+      <c r="GG5" s="3"/>
+      <c r="GH5" s="3"/>
+      <c r="GI5" s="3"/>
+      <c r="GJ5" s="3"/>
+      <c r="GK5" s="3"/>
+      <c r="GL5" s="3"/>
+      <c r="GM5" s="3"/>
+      <c r="GN5" s="3"/>
+      <c r="GO5" s="3"/>
+      <c r="GP5" s="3"/>
+      <c r="GQ5" s="3"/>
+      <c r="GR5" s="3"/>
+      <c r="GS5" s="3"/>
+      <c r="GT5" s="3"/>
+      <c r="GU5" s="3"/>
+      <c r="GV5" s="3"/>
+      <c r="GW5" s="3"/>
+      <c r="GX5" s="3"/>
+      <c r="GY5" s="3"/>
+      <c r="GZ5" s="3"/>
+      <c r="HA5" s="3"/>
+      <c r="HB5" s="3"/>
+      <c r="HC5" s="3"/>
+      <c r="HD5" s="3"/>
+      <c r="HE5" s="3"/>
+      <c r="HF5" s="3"/>
+      <c r="HG5" s="3"/>
+      <c r="HH5" s="3"/>
+      <c r="HI5" s="3"/>
+      <c r="HJ5" s="3"/>
+      <c r="HK5" s="3"/>
+      <c r="HL5" s="3"/>
+      <c r="HM5" s="3"/>
+      <c r="HN5" s="3"/>
+      <c r="HO5" s="3"/>
+      <c r="HP5" s="3"/>
+      <c r="HQ5" s="3"/>
+      <c r="HR5" s="3"/>
+      <c r="HS5" s="3"/>
+      <c r="HT5" s="3"/>
+      <c r="HU5" s="3"/>
+      <c r="HV5" s="3"/>
+      <c r="HW5" s="3"/>
+      <c r="HX5" s="3"/>
+      <c r="HY5" s="3"/>
+      <c r="HZ5" s="3"/>
+      <c r="IA5" s="3"/>
+      <c r="IB5" s="3"/>
+      <c r="IC5" s="3"/>
+      <c r="ID5" s="3"/>
+      <c r="IE5" s="3"/>
+      <c r="IF5" s="3"/>
+      <c r="IG5" s="3"/>
+      <c r="IH5" s="3"/>
+      <c r="II5" s="3"/>
+      <c r="IJ5" s="3"/>
+      <c r="IK5" s="3"/>
+      <c r="IL5" s="3"/>
+      <c r="IM5" s="3"/>
+      <c r="IN5" s="3"/>
+      <c r="IO5" s="3"/>
+      <c r="IP5" s="3"/>
+      <c r="IQ5" s="3"/>
+      <c r="IR5" s="3"/>
+      <c r="IS5" s="3"/>
+      <c r="IT5" s="3"/>
+      <c r="IU5" s="3"/>
+      <c r="IV5" s="3"/>
+      <c r="IW5" s="3"/>
+      <c r="IX5" s="3"/>
+      <c r="IY5" s="3"/>
+      <c r="IZ5" s="3"/>
+      <c r="JA5" s="3"/>
+      <c r="JB5" s="3"/>
+      <c r="JC5" s="3"/>
+      <c r="JD5" s="3"/>
+      <c r="JE5" s="3"/>
+      <c r="JF5" s="3"/>
+      <c r="JG5" s="3"/>
+      <c r="JH5" s="3"/>
+      <c r="JI5" s="3"/>
+      <c r="JJ5" s="3"/>
+      <c r="JK5" s="3"/>
+      <c r="JL5" s="3"/>
+      <c r="JM5" s="3"/>
+      <c r="JN5" s="3"/>
+      <c r="JO5" s="3"/>
+      <c r="JP5" s="3"/>
+      <c r="JQ5" s="3"/>
+      <c r="JR5" s="3"/>
+      <c r="JS5" s="3"/>
+      <c r="JT5" s="3"/>
+      <c r="JU5" s="3"/>
+      <c r="JV5" s="3"/>
+      <c r="JW5" s="3"/>
+      <c r="JX5" s="3"/>
+      <c r="JY5" s="3"/>
+      <c r="JZ5" s="3"/>
+      <c r="KA5" s="3"/>
+      <c r="KB5" s="3"/>
+      <c r="KC5" s="3"/>
+      <c r="KD5" s="3"/>
+      <c r="KE5" s="3"/>
+      <c r="KF5" s="3"/>
+      <c r="KG5" s="3"/>
+      <c r="KH5" s="3"/>
+      <c r="KI5" s="3"/>
+      <c r="KJ5" s="3"/>
+      <c r="KK5" s="3"/>
+      <c r="KL5" s="3"/>
+      <c r="KM5" s="3"/>
+      <c r="KN5" s="3"/>
+      <c r="KO5" s="3"/>
+      <c r="KP5" s="3"/>
+      <c r="KQ5" s="3"/>
+      <c r="KR5" s="3"/>
+      <c r="KS5" s="3"/>
+      <c r="KT5" s="3"/>
+      <c r="KU5" s="3"/>
+      <c r="KV5" s="3"/>
+      <c r="KW5" s="3"/>
+      <c r="KX5" s="3"/>
+      <c r="KY5" s="3"/>
+      <c r="KZ5" s="3"/>
+      <c r="LA5" s="3"/>
+      <c r="LB5" s="3"/>
+      <c r="LC5" s="3"/>
+      <c r="LD5" s="3"/>
+      <c r="LE5" s="3"/>
+      <c r="LF5" s="3"/>
+      <c r="LG5" s="3"/>
+      <c r="LH5" s="3"/>
+      <c r="LI5" s="3"/>
+      <c r="LJ5" s="3"/>
+      <c r="LK5" s="3"/>
+      <c r="LL5" s="3"/>
+      <c r="LM5" s="3"/>
+      <c r="LN5" s="3"/>
+      <c r="LO5" s="3"/>
+      <c r="LP5" s="3"/>
+      <c r="LQ5" s="3"/>
+      <c r="LR5" s="3"/>
+      <c r="LS5" s="3"/>
+      <c r="LT5" s="3"/>
+      <c r="LU5" s="3"/>
+      <c r="LV5" s="3"/>
+      <c r="LW5" s="3"/>
+      <c r="LX5" s="3"/>
+      <c r="LY5" s="3"/>
+      <c r="LZ5" s="3"/>
+      <c r="MA5" s="3"/>
+      <c r="MB5" s="3"/>
+      <c r="MC5" s="3"/>
+      <c r="MD5" s="3"/>
+      <c r="ME5" s="3"/>
+      <c r="MF5" s="3"/>
+      <c r="MG5" s="3"/>
+      <c r="MH5" s="3"/>
+      <c r="MI5" s="3"/>
+      <c r="MJ5" s="3"/>
+      <c r="MK5" s="3"/>
+      <c r="ML5" s="3"/>
+      <c r="MM5" s="3"/>
+      <c r="MN5" s="3"/>
+      <c r="MO5" s="3"/>
+      <c r="MP5" s="3"/>
+      <c r="MQ5" s="3"/>
+      <c r="MR5" s="3"/>
+      <c r="MS5" s="3"/>
+      <c r="MT5" s="3"/>
+      <c r="MU5" s="3"/>
+      <c r="MV5" s="3"/>
+      <c r="MW5" s="3"/>
+      <c r="MX5" s="3"/>
+      <c r="MY5" s="3"/>
+      <c r="MZ5" s="3"/>
+      <c r="NA5" s="3"/>
+      <c r="NB5" s="3"/>
+      <c r="NC5" s="3"/>
+      <c r="ND5" s="3"/>
+      <c r="NE5" s="3"/>
+      <c r="NF5" s="3"/>
+      <c r="NG5" s="3"/>
+      <c r="NH5" s="3"/>
+      <c r="NI5" s="3"/>
+      <c r="NJ5" s="3"/>
+      <c r="NK5" s="3"/>
+      <c r="NL5" s="3"/>
+      <c r="NM5" s="3"/>
+      <c r="NN5" s="3"/>
+      <c r="NO5" s="3"/>
+      <c r="NP5" s="3"/>
+      <c r="NQ5" s="3"/>
+      <c r="NR5" s="3"/>
+      <c r="NS5" s="3"/>
+      <c r="NT5" s="3"/>
+      <c r="NU5" s="3"/>
+      <c r="NV5" s="3"/>
+      <c r="NW5" s="3"/>
+      <c r="NX5" s="3"/>
+      <c r="NY5" s="3"/>
+      <c r="NZ5" s="3"/>
+      <c r="OA5" s="3"/>
+      <c r="OB5" s="3"/>
+      <c r="OC5" s="3"/>
+      <c r="OD5" s="3"/>
+      <c r="OE5" s="3"/>
+      <c r="OF5" s="3"/>
+      <c r="OG5" s="3"/>
+      <c r="OH5" s="3"/>
+      <c r="OI5" s="3"/>
+      <c r="OJ5" s="3"/>
+      <c r="OK5" s="3"/>
+      <c r="OL5" s="3"/>
+      <c r="OM5" s="3"/>
+      <c r="ON5" s="3"/>
+      <c r="OO5" s="3"/>
+      <c r="OP5" s="3"/>
+      <c r="OQ5" s="3"/>
+      <c r="OR5" s="3"/>
+      <c r="OS5" s="3"/>
+      <c r="OT5" s="3"/>
+      <c r="OU5" s="3"/>
+      <c r="OV5" s="3"/>
+      <c r="OW5" s="3"/>
+      <c r="OX5" s="3"/>
+      <c r="OY5" s="3"/>
+      <c r="OZ5" s="3"/>
+      <c r="PA5" s="3"/>
+      <c r="PB5" s="3"/>
+      <c r="PC5" s="3"/>
+      <c r="PD5" s="3"/>
+      <c r="PE5" s="3"/>
+      <c r="PF5" s="3"/>
+      <c r="PG5" s="3"/>
+      <c r="PH5" s="3"/>
+      <c r="PI5" s="3"/>
+      <c r="PJ5" s="3"/>
+      <c r="PK5" s="3"/>
+      <c r="PL5" s="3"/>
+      <c r="PM5" s="3"/>
+      <c r="PN5" s="3"/>
+      <c r="PO5" s="3"/>
+      <c r="PP5" s="3"/>
+      <c r="PQ5" s="3"/>
+      <c r="PR5" s="3"/>
+      <c r="PS5" s="3"/>
+      <c r="PT5" s="3"/>
+      <c r="PU5" s="3"/>
+      <c r="PV5" s="3"/>
+      <c r="PW5" s="3"/>
+      <c r="PX5" s="3"/>
+      <c r="PY5" s="3"/>
+      <c r="PZ5" s="3"/>
+      <c r="QA5" s="3"/>
+      <c r="QB5" s="3"/>
+      <c r="QC5" s="3"/>
+      <c r="QD5" s="3"/>
+      <c r="QE5" s="3"/>
+      <c r="QF5" s="3"/>
+      <c r="QG5" s="3"/>
+      <c r="QH5" s="3"/>
+      <c r="QI5" s="3"/>
+      <c r="QJ5" s="3"/>
+      <c r="QK5" s="3"/>
+      <c r="QL5" s="3"/>
+      <c r="QM5" s="3"/>
+      <c r="QN5" s="3"/>
+      <c r="QO5" s="3"/>
+      <c r="QP5" s="3"/>
+      <c r="QQ5" s="3"/>
     </row>
     <row r="6" spans="1:459" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1761,7 +1793,7 @@
       <c r="E6">
         <v>39.5</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H6">
@@ -1790,7 +1822,7 @@
       <c r="E7">
         <v>35.700000000000003</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H7">
@@ -1819,7 +1851,7 @@
       <c r="E8">
         <v>16.3</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H8">
@@ -1848,7 +1880,7 @@
       <c r="E9">
         <v>16.7</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="H9">
@@ -1877,7 +1909,7 @@
       <c r="E10">
         <v>23.4</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H10">
@@ -1906,7 +1938,7 @@
       <c r="E11">
         <v>18.3</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>37</v>
       </c>
       <c r="H11">
@@ -1935,7 +1967,7 @@
       <c r="E12">
         <v>35.200000000000003</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="10" t="s">
         <v>38</v>
       </c>
       <c r="H12">
@@ -1949,18 +1981,18 @@
       </c>
     </row>
     <row r="14" spans="1:459" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="G14" s="1" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="G14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:459" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2004,7 +2036,7 @@
       <c r="E16">
         <v>26.5</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="23" t="s">
         <v>52</v>
       </c>
       <c r="H16">
@@ -2033,7 +2065,7 @@
       <c r="E17">
         <v>30.1</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="11" t="s">
         <v>41</v>
       </c>
       <c r="H17">
@@ -2062,7 +2094,7 @@
       <c r="E18">
         <v>19.600000000000001</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="12" t="s">
         <v>42</v>
       </c>
       <c r="H18">
@@ -2091,7 +2123,7 @@
       <c r="E19">
         <v>7.7</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>44</v>
       </c>
       <c r="H19">
@@ -2120,7 +2152,7 @@
       <c r="E20">
         <v>13.6</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="13" t="s">
         <v>43</v>
       </c>
       <c r="H20">
@@ -2149,7 +2181,7 @@
       <c r="E21">
         <v>9.5</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H21">
@@ -2178,7 +2210,7 @@
       <c r="E22">
         <v>8.6</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="16" t="s">
         <v>46</v>
       </c>
       <c r="H22">
@@ -2207,7 +2239,7 @@
       <c r="E23">
         <v>11.3</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="22" t="s">
         <v>51</v>
       </c>
       <c r="H23">
@@ -2236,7 +2268,7 @@
       <c r="E24">
         <v>18.7</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="19" t="s">
         <v>49</v>
       </c>
       <c r="H24">
@@ -2265,7 +2297,7 @@
       <c r="E25">
         <v>12.8</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="20" t="s">
         <v>50</v>
       </c>
       <c r="H25">
@@ -2294,7 +2326,7 @@
       <c r="E26">
         <v>15</v>
       </c>
-      <c r="G26" s="23" t="s">
+      <c r="G26" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H26">
@@ -2323,7 +2355,7 @@
       <c r="E27">
         <v>15.5</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="17" t="s">
         <v>47</v>
       </c>
       <c r="H27">
@@ -2352,7 +2384,7 @@
       <c r="E28">
         <v>11.7</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="18" t="s">
         <v>48</v>
       </c>
       <c r="H28">
@@ -2363,6 +2395,281 @@
       </c>
       <c r="J28">
         <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="23">
+        <v>16.3</v>
+      </c>
+      <c r="C32" s="26">
+        <f>B32*(10^6)/3600</f>
+        <v>4527.7777777777774</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="23">
+        <v>9.5</v>
+      </c>
+      <c r="C33" s="26">
+        <f t="shared" ref="C33:C53" si="0">B33*(10^6)/3600</f>
+        <v>2638.8888888888887</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="23">
+        <v>16.7</v>
+      </c>
+      <c r="C34" s="26">
+        <f t="shared" si="0"/>
+        <v>4638.8888888888887</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="23">
+        <v>18.2</v>
+      </c>
+      <c r="C35" s="26">
+        <f t="shared" si="0"/>
+        <v>5055.5555555555557</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="23">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="C36" s="26">
+        <f t="shared" si="0"/>
+        <v>5444.4444444444443</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="23">
+        <v>23.4</v>
+      </c>
+      <c r="C37" s="26">
+        <f t="shared" si="0"/>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="23">
+        <v>18.3</v>
+      </c>
+      <c r="C38" s="26">
+        <f t="shared" si="0"/>
+        <v>5083.333333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="23">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="C39" s="26">
+        <f t="shared" si="0"/>
+        <v>9916.6666666666661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="23">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="C40" s="26">
+        <f t="shared" si="0"/>
+        <v>9777.7777777777774</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="23">
+        <v>30.1</v>
+      </c>
+      <c r="C41" s="26">
+        <f t="shared" si="0"/>
+        <v>8361.1111111111113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="23">
+        <v>39.5</v>
+      </c>
+      <c r="C42" s="26">
+        <f t="shared" si="0"/>
+        <v>10972.222222222223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="23">
+        <v>15</v>
+      </c>
+      <c r="C43" s="26">
+        <f t="shared" si="0"/>
+        <v>4166.666666666667</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="23">
+        <v>15.5</v>
+      </c>
+      <c r="C44" s="26">
+        <f t="shared" si="0"/>
+        <v>4305.5555555555557</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="23">
+        <v>11.3</v>
+      </c>
+      <c r="C45" s="26">
+        <f t="shared" si="0"/>
+        <v>3138.8888888888887</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="23">
+        <v>18.7</v>
+      </c>
+      <c r="C46" s="26">
+        <f t="shared" si="0"/>
+        <v>5194.4444444444443</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="23">
+        <v>11.7</v>
+      </c>
+      <c r="C47" s="26">
+        <f t="shared" si="0"/>
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="23">
+        <v>9.5</v>
+      </c>
+      <c r="C48" s="26">
+        <f t="shared" si="0"/>
+        <v>2638.8888888888887</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="23">
+        <v>7.7</v>
+      </c>
+      <c r="C49" s="26">
+        <f t="shared" si="0"/>
+        <v>2138.8888888888887</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="23">
+        <v>13.6</v>
+      </c>
+      <c r="C50" s="26">
+        <f t="shared" si="0"/>
+        <v>3777.7777777777778</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="23">
+        <v>26.5</v>
+      </c>
+      <c r="C51" s="26">
+        <f t="shared" si="0"/>
+        <v>7361.1111111111113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="23">
+        <v>12.8</v>
+      </c>
+      <c r="C52" s="26">
+        <f t="shared" si="0"/>
+        <v>3555.5555555555557</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="23">
+        <v>8.6</v>
+      </c>
+      <c r="C53" s="26">
+        <f t="shared" si="0"/>
+        <v>2388.8888888888887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "WORK IN PROGRESS: Updating the TV input data, and preparing to add a miscellaneous baseload."
This reverts commit 492f03a7868795b9349c3bdb358000adb7904a6d.
</commit_message>
<xml_diff>
--- a/bcd/CREST/ValidationSet.xlsx
+++ b/bcd/CREST/ValidationSet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Record</t>
   </si>
@@ -271,33 +271,6 @@
   </si>
   <si>
     <t>non-HVAC [GJ]</t>
-  </si>
-  <si>
-    <t>H01</t>
-  </si>
-  <si>
-    <t>H02</t>
-  </si>
-  <si>
-    <t>H03</t>
-  </si>
-  <si>
-    <t>H04</t>
-  </si>
-  <si>
-    <t>H05</t>
-  </si>
-  <si>
-    <t>H06</t>
-  </si>
-  <si>
-    <t>H07</t>
-  </si>
-  <si>
-    <t>H09</t>
-  </si>
-  <si>
-    <t>non-HVAC [kWh]</t>
   </si>
 </sst>
 </file>
@@ -815,8 +788,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,17 +821,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1195,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:QQ53"/>
+  <dimension ref="A1:QQ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,42 +1174,42 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="6" max="6" width="9.140625" style="25"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:459" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:459" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:459" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1256,7 +1224,7 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
@@ -1271,7 +1239,7 @@
       <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1320,462 +1288,462 @@
       <c r="E5">
         <v>18.2</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="5">
         <v>1953</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="5">
         <v>165.54</v>
       </c>
       <c r="J5">
         <v>4</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
-      <c r="AO5" s="3"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="3"/>
-      <c r="AR5" s="3"/>
-      <c r="AS5" s="3"/>
-      <c r="AT5" s="3"/>
-      <c r="AU5" s="3"/>
-      <c r="AV5" s="3"/>
-      <c r="AW5" s="3"/>
-      <c r="AX5" s="3"/>
-      <c r="AY5" s="3"/>
-      <c r="AZ5" s="3"/>
-      <c r="BA5" s="3"/>
-      <c r="BB5" s="3"/>
-      <c r="BC5" s="3"/>
-      <c r="BD5" s="3"/>
-      <c r="BE5" s="3"/>
-      <c r="BF5" s="3"/>
-      <c r="BG5" s="3"/>
-      <c r="BH5" s="3"/>
-      <c r="BI5" s="3"/>
-      <c r="BJ5" s="3"/>
-      <c r="BK5" s="3"/>
-      <c r="BL5" s="3"/>
-      <c r="BM5" s="3"/>
-      <c r="BN5" s="3"/>
-      <c r="BO5" s="3"/>
-      <c r="BP5" s="3"/>
-      <c r="BQ5" s="3"/>
-      <c r="BR5" s="3"/>
-      <c r="BS5" s="3"/>
-      <c r="BT5" s="3"/>
-      <c r="BU5" s="3"/>
-      <c r="BV5" s="3"/>
-      <c r="BW5" s="3"/>
-      <c r="BX5" s="3"/>
-      <c r="BY5" s="3"/>
-      <c r="BZ5" s="3"/>
-      <c r="CA5" s="3"/>
-      <c r="CB5" s="3"/>
-      <c r="CC5" s="3"/>
-      <c r="CD5" s="3"/>
-      <c r="CE5" s="3"/>
-      <c r="CF5" s="3"/>
-      <c r="CG5" s="3"/>
-      <c r="CH5" s="3"/>
-      <c r="CI5" s="3"/>
-      <c r="CJ5" s="3"/>
-      <c r="CK5" s="3"/>
-      <c r="CL5" s="3"/>
-      <c r="CM5" s="3"/>
-      <c r="CN5" s="3"/>
-      <c r="CO5" s="3"/>
-      <c r="CP5" s="3"/>
-      <c r="CQ5" s="3"/>
-      <c r="CR5" s="3"/>
-      <c r="CS5" s="3"/>
-      <c r="CT5" s="3"/>
-      <c r="CU5" s="3"/>
-      <c r="CV5" s="3"/>
-      <c r="CW5" s="3"/>
-      <c r="CX5" s="3"/>
-      <c r="CY5" s="3"/>
-      <c r="CZ5" s="3"/>
-      <c r="DA5" s="3"/>
-      <c r="DB5" s="3"/>
-      <c r="DC5" s="3"/>
-      <c r="DD5" s="3"/>
-      <c r="DE5" s="3"/>
-      <c r="DF5" s="3"/>
-      <c r="DG5" s="3"/>
-      <c r="DH5" s="3"/>
-      <c r="DI5" s="3"/>
-      <c r="DJ5" s="3"/>
-      <c r="DK5" s="3"/>
-      <c r="DL5" s="3"/>
-      <c r="DM5" s="3"/>
-      <c r="DN5" s="3"/>
-      <c r="DO5" s="3"/>
-      <c r="DP5" s="3"/>
-      <c r="DQ5" s="3"/>
-      <c r="DR5" s="3"/>
-      <c r="DS5" s="3"/>
-      <c r="DT5" s="3"/>
-      <c r="DU5" s="3"/>
-      <c r="DV5" s="3"/>
-      <c r="DW5" s="3"/>
-      <c r="DX5" s="3"/>
-      <c r="DY5" s="3"/>
-      <c r="DZ5" s="3"/>
-      <c r="EA5" s="3"/>
-      <c r="EB5" s="3"/>
-      <c r="EC5" s="3"/>
-      <c r="ED5" s="3"/>
-      <c r="EE5" s="3"/>
-      <c r="EF5" s="3"/>
-      <c r="EG5" s="3"/>
-      <c r="EH5" s="3"/>
-      <c r="EI5" s="3"/>
-      <c r="EJ5" s="3"/>
-      <c r="EK5" s="3"/>
-      <c r="EL5" s="3"/>
-      <c r="EM5" s="3"/>
-      <c r="EN5" s="3"/>
-      <c r="EO5" s="3"/>
-      <c r="EP5" s="3"/>
-      <c r="EQ5" s="3"/>
-      <c r="ER5" s="3"/>
-      <c r="ES5" s="3"/>
-      <c r="ET5" s="3"/>
-      <c r="EU5" s="3"/>
-      <c r="EV5" s="3"/>
-      <c r="EW5" s="3"/>
-      <c r="EX5" s="3"/>
-      <c r="EY5" s="3"/>
-      <c r="EZ5" s="3"/>
-      <c r="FA5" s="3"/>
-      <c r="FB5" s="3"/>
-      <c r="FC5" s="3"/>
-      <c r="FD5" s="3"/>
-      <c r="FE5" s="3"/>
-      <c r="FF5" s="3"/>
-      <c r="FG5" s="3"/>
-      <c r="FH5" s="3"/>
-      <c r="FI5" s="3"/>
-      <c r="FJ5" s="3"/>
-      <c r="FK5" s="3"/>
-      <c r="FL5" s="3"/>
-      <c r="FM5" s="3"/>
-      <c r="FN5" s="3"/>
-      <c r="FO5" s="3"/>
-      <c r="FP5" s="3"/>
-      <c r="FQ5" s="3"/>
-      <c r="FR5" s="3"/>
-      <c r="FS5" s="3"/>
-      <c r="FT5" s="3"/>
-      <c r="FU5" s="3"/>
-      <c r="FV5" s="3"/>
-      <c r="FW5" s="3"/>
-      <c r="FX5" s="3"/>
-      <c r="FY5" s="3"/>
-      <c r="FZ5" s="3"/>
-      <c r="GA5" s="3"/>
-      <c r="GB5" s="3"/>
-      <c r="GC5" s="3"/>
-      <c r="GD5" s="3"/>
-      <c r="GE5" s="3"/>
-      <c r="GF5" s="3"/>
-      <c r="GG5" s="3"/>
-      <c r="GH5" s="3"/>
-      <c r="GI5" s="3"/>
-      <c r="GJ5" s="3"/>
-      <c r="GK5" s="3"/>
-      <c r="GL5" s="3"/>
-      <c r="GM5" s="3"/>
-      <c r="GN5" s="3"/>
-      <c r="GO5" s="3"/>
-      <c r="GP5" s="3"/>
-      <c r="GQ5" s="3"/>
-      <c r="GR5" s="3"/>
-      <c r="GS5" s="3"/>
-      <c r="GT5" s="3"/>
-      <c r="GU5" s="3"/>
-      <c r="GV5" s="3"/>
-      <c r="GW5" s="3"/>
-      <c r="GX5" s="3"/>
-      <c r="GY5" s="3"/>
-      <c r="GZ5" s="3"/>
-      <c r="HA5" s="3"/>
-      <c r="HB5" s="3"/>
-      <c r="HC5" s="3"/>
-      <c r="HD5" s="3"/>
-      <c r="HE5" s="3"/>
-      <c r="HF5" s="3"/>
-      <c r="HG5" s="3"/>
-      <c r="HH5" s="3"/>
-      <c r="HI5" s="3"/>
-      <c r="HJ5" s="3"/>
-      <c r="HK5" s="3"/>
-      <c r="HL5" s="3"/>
-      <c r="HM5" s="3"/>
-      <c r="HN5" s="3"/>
-      <c r="HO5" s="3"/>
-      <c r="HP5" s="3"/>
-      <c r="HQ5" s="3"/>
-      <c r="HR5" s="3"/>
-      <c r="HS5" s="3"/>
-      <c r="HT5" s="3"/>
-      <c r="HU5" s="3"/>
-      <c r="HV5" s="3"/>
-      <c r="HW5" s="3"/>
-      <c r="HX5" s="3"/>
-      <c r="HY5" s="3"/>
-      <c r="HZ5" s="3"/>
-      <c r="IA5" s="3"/>
-      <c r="IB5" s="3"/>
-      <c r="IC5" s="3"/>
-      <c r="ID5" s="3"/>
-      <c r="IE5" s="3"/>
-      <c r="IF5" s="3"/>
-      <c r="IG5" s="3"/>
-      <c r="IH5" s="3"/>
-      <c r="II5" s="3"/>
-      <c r="IJ5" s="3"/>
-      <c r="IK5" s="3"/>
-      <c r="IL5" s="3"/>
-      <c r="IM5" s="3"/>
-      <c r="IN5" s="3"/>
-      <c r="IO5" s="3"/>
-      <c r="IP5" s="3"/>
-      <c r="IQ5" s="3"/>
-      <c r="IR5" s="3"/>
-      <c r="IS5" s="3"/>
-      <c r="IT5" s="3"/>
-      <c r="IU5" s="3"/>
-      <c r="IV5" s="3"/>
-      <c r="IW5" s="3"/>
-      <c r="IX5" s="3"/>
-      <c r="IY5" s="3"/>
-      <c r="IZ5" s="3"/>
-      <c r="JA5" s="3"/>
-      <c r="JB5" s="3"/>
-      <c r="JC5" s="3"/>
-      <c r="JD5" s="3"/>
-      <c r="JE5" s="3"/>
-      <c r="JF5" s="3"/>
-      <c r="JG5" s="3"/>
-      <c r="JH5" s="3"/>
-      <c r="JI5" s="3"/>
-      <c r="JJ5" s="3"/>
-      <c r="JK5" s="3"/>
-      <c r="JL5" s="3"/>
-      <c r="JM5" s="3"/>
-      <c r="JN5" s="3"/>
-      <c r="JO5" s="3"/>
-      <c r="JP5" s="3"/>
-      <c r="JQ5" s="3"/>
-      <c r="JR5" s="3"/>
-      <c r="JS5" s="3"/>
-      <c r="JT5" s="3"/>
-      <c r="JU5" s="3"/>
-      <c r="JV5" s="3"/>
-      <c r="JW5" s="3"/>
-      <c r="JX5" s="3"/>
-      <c r="JY5" s="3"/>
-      <c r="JZ5" s="3"/>
-      <c r="KA5" s="3"/>
-      <c r="KB5" s="3"/>
-      <c r="KC5" s="3"/>
-      <c r="KD5" s="3"/>
-      <c r="KE5" s="3"/>
-      <c r="KF5" s="3"/>
-      <c r="KG5" s="3"/>
-      <c r="KH5" s="3"/>
-      <c r="KI5" s="3"/>
-      <c r="KJ5" s="3"/>
-      <c r="KK5" s="3"/>
-      <c r="KL5" s="3"/>
-      <c r="KM5" s="3"/>
-      <c r="KN5" s="3"/>
-      <c r="KO5" s="3"/>
-      <c r="KP5" s="3"/>
-      <c r="KQ5" s="3"/>
-      <c r="KR5" s="3"/>
-      <c r="KS5" s="3"/>
-      <c r="KT5" s="3"/>
-      <c r="KU5" s="3"/>
-      <c r="KV5" s="3"/>
-      <c r="KW5" s="3"/>
-      <c r="KX5" s="3"/>
-      <c r="KY5" s="3"/>
-      <c r="KZ5" s="3"/>
-      <c r="LA5" s="3"/>
-      <c r="LB5" s="3"/>
-      <c r="LC5" s="3"/>
-      <c r="LD5" s="3"/>
-      <c r="LE5" s="3"/>
-      <c r="LF5" s="3"/>
-      <c r="LG5" s="3"/>
-      <c r="LH5" s="3"/>
-      <c r="LI5" s="3"/>
-      <c r="LJ5" s="3"/>
-      <c r="LK5" s="3"/>
-      <c r="LL5" s="3"/>
-      <c r="LM5" s="3"/>
-      <c r="LN5" s="3"/>
-      <c r="LO5" s="3"/>
-      <c r="LP5" s="3"/>
-      <c r="LQ5" s="3"/>
-      <c r="LR5" s="3"/>
-      <c r="LS5" s="3"/>
-      <c r="LT5" s="3"/>
-      <c r="LU5" s="3"/>
-      <c r="LV5" s="3"/>
-      <c r="LW5" s="3"/>
-      <c r="LX5" s="3"/>
-      <c r="LY5" s="3"/>
-      <c r="LZ5" s="3"/>
-      <c r="MA5" s="3"/>
-      <c r="MB5" s="3"/>
-      <c r="MC5" s="3"/>
-      <c r="MD5" s="3"/>
-      <c r="ME5" s="3"/>
-      <c r="MF5" s="3"/>
-      <c r="MG5" s="3"/>
-      <c r="MH5" s="3"/>
-      <c r="MI5" s="3"/>
-      <c r="MJ5" s="3"/>
-      <c r="MK5" s="3"/>
-      <c r="ML5" s="3"/>
-      <c r="MM5" s="3"/>
-      <c r="MN5" s="3"/>
-      <c r="MO5" s="3"/>
-      <c r="MP5" s="3"/>
-      <c r="MQ5" s="3"/>
-      <c r="MR5" s="3"/>
-      <c r="MS5" s="3"/>
-      <c r="MT5" s="3"/>
-      <c r="MU5" s="3"/>
-      <c r="MV5" s="3"/>
-      <c r="MW5" s="3"/>
-      <c r="MX5" s="3"/>
-      <c r="MY5" s="3"/>
-      <c r="MZ5" s="3"/>
-      <c r="NA5" s="3"/>
-      <c r="NB5" s="3"/>
-      <c r="NC5" s="3"/>
-      <c r="ND5" s="3"/>
-      <c r="NE5" s="3"/>
-      <c r="NF5" s="3"/>
-      <c r="NG5" s="3"/>
-      <c r="NH5" s="3"/>
-      <c r="NI5" s="3"/>
-      <c r="NJ5" s="3"/>
-      <c r="NK5" s="3"/>
-      <c r="NL5" s="3"/>
-      <c r="NM5" s="3"/>
-      <c r="NN5" s="3"/>
-      <c r="NO5" s="3"/>
-      <c r="NP5" s="3"/>
-      <c r="NQ5" s="3"/>
-      <c r="NR5" s="3"/>
-      <c r="NS5" s="3"/>
-      <c r="NT5" s="3"/>
-      <c r="NU5" s="3"/>
-      <c r="NV5" s="3"/>
-      <c r="NW5" s="3"/>
-      <c r="NX5" s="3"/>
-      <c r="NY5" s="3"/>
-      <c r="NZ5" s="3"/>
-      <c r="OA5" s="3"/>
-      <c r="OB5" s="3"/>
-      <c r="OC5" s="3"/>
-      <c r="OD5" s="3"/>
-      <c r="OE5" s="3"/>
-      <c r="OF5" s="3"/>
-      <c r="OG5" s="3"/>
-      <c r="OH5" s="3"/>
-      <c r="OI5" s="3"/>
-      <c r="OJ5" s="3"/>
-      <c r="OK5" s="3"/>
-      <c r="OL5" s="3"/>
-      <c r="OM5" s="3"/>
-      <c r="ON5" s="3"/>
-      <c r="OO5" s="3"/>
-      <c r="OP5" s="3"/>
-      <c r="OQ5" s="3"/>
-      <c r="OR5" s="3"/>
-      <c r="OS5" s="3"/>
-      <c r="OT5" s="3"/>
-      <c r="OU5" s="3"/>
-      <c r="OV5" s="3"/>
-      <c r="OW5" s="3"/>
-      <c r="OX5" s="3"/>
-      <c r="OY5" s="3"/>
-      <c r="OZ5" s="3"/>
-      <c r="PA5" s="3"/>
-      <c r="PB5" s="3"/>
-      <c r="PC5" s="3"/>
-      <c r="PD5" s="3"/>
-      <c r="PE5" s="3"/>
-      <c r="PF5" s="3"/>
-      <c r="PG5" s="3"/>
-      <c r="PH5" s="3"/>
-      <c r="PI5" s="3"/>
-      <c r="PJ5" s="3"/>
-      <c r="PK5" s="3"/>
-      <c r="PL5" s="3"/>
-      <c r="PM5" s="3"/>
-      <c r="PN5" s="3"/>
-      <c r="PO5" s="3"/>
-      <c r="PP5" s="3"/>
-      <c r="PQ5" s="3"/>
-      <c r="PR5" s="3"/>
-      <c r="PS5" s="3"/>
-      <c r="PT5" s="3"/>
-      <c r="PU5" s="3"/>
-      <c r="PV5" s="3"/>
-      <c r="PW5" s="3"/>
-      <c r="PX5" s="3"/>
-      <c r="PY5" s="3"/>
-      <c r="PZ5" s="3"/>
-      <c r="QA5" s="3"/>
-      <c r="QB5" s="3"/>
-      <c r="QC5" s="3"/>
-      <c r="QD5" s="3"/>
-      <c r="QE5" s="3"/>
-      <c r="QF5" s="3"/>
-      <c r="QG5" s="3"/>
-      <c r="QH5" s="3"/>
-      <c r="QI5" s="3"/>
-      <c r="QJ5" s="3"/>
-      <c r="QK5" s="3"/>
-      <c r="QL5" s="3"/>
-      <c r="QM5" s="3"/>
-      <c r="QN5" s="3"/>
-      <c r="QO5" s="3"/>
-      <c r="QP5" s="3"/>
-      <c r="QQ5" s="3"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="5"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="5"/>
+      <c r="BD5" s="5"/>
+      <c r="BE5" s="5"/>
+      <c r="BF5" s="5"/>
+      <c r="BG5" s="5"/>
+      <c r="BH5" s="5"/>
+      <c r="BI5" s="5"/>
+      <c r="BJ5" s="5"/>
+      <c r="BK5" s="5"/>
+      <c r="BL5" s="5"/>
+      <c r="BM5" s="5"/>
+      <c r="BN5" s="5"/>
+      <c r="BO5" s="5"/>
+      <c r="BP5" s="5"/>
+      <c r="BQ5" s="5"/>
+      <c r="BR5" s="5"/>
+      <c r="BS5" s="5"/>
+      <c r="BT5" s="5"/>
+      <c r="BU5" s="5"/>
+      <c r="BV5" s="5"/>
+      <c r="BW5" s="5"/>
+      <c r="BX5" s="5"/>
+      <c r="BY5" s="5"/>
+      <c r="BZ5" s="5"/>
+      <c r="CA5" s="5"/>
+      <c r="CB5" s="5"/>
+      <c r="CC5" s="5"/>
+      <c r="CD5" s="5"/>
+      <c r="CE5" s="5"/>
+      <c r="CF5" s="5"/>
+      <c r="CG5" s="5"/>
+      <c r="CH5" s="5"/>
+      <c r="CI5" s="5"/>
+      <c r="CJ5" s="5"/>
+      <c r="CK5" s="5"/>
+      <c r="CL5" s="5"/>
+      <c r="CM5" s="5"/>
+      <c r="CN5" s="5"/>
+      <c r="CO5" s="5"/>
+      <c r="CP5" s="5"/>
+      <c r="CQ5" s="5"/>
+      <c r="CR5" s="5"/>
+      <c r="CS5" s="5"/>
+      <c r="CT5" s="5"/>
+      <c r="CU5" s="5"/>
+      <c r="CV5" s="5"/>
+      <c r="CW5" s="5"/>
+      <c r="CX5" s="5"/>
+      <c r="CY5" s="5"/>
+      <c r="CZ5" s="5"/>
+      <c r="DA5" s="5"/>
+      <c r="DB5" s="5"/>
+      <c r="DC5" s="5"/>
+      <c r="DD5" s="5"/>
+      <c r="DE5" s="5"/>
+      <c r="DF5" s="5"/>
+      <c r="DG5" s="5"/>
+      <c r="DH5" s="5"/>
+      <c r="DI5" s="5"/>
+      <c r="DJ5" s="5"/>
+      <c r="DK5" s="5"/>
+      <c r="DL5" s="5"/>
+      <c r="DM5" s="5"/>
+      <c r="DN5" s="5"/>
+      <c r="DO5" s="5"/>
+      <c r="DP5" s="5"/>
+      <c r="DQ5" s="5"/>
+      <c r="DR5" s="5"/>
+      <c r="DS5" s="5"/>
+      <c r="DT5" s="5"/>
+      <c r="DU5" s="5"/>
+      <c r="DV5" s="5"/>
+      <c r="DW5" s="5"/>
+      <c r="DX5" s="5"/>
+      <c r="DY5" s="5"/>
+      <c r="DZ5" s="5"/>
+      <c r="EA5" s="5"/>
+      <c r="EB5" s="5"/>
+      <c r="EC5" s="5"/>
+      <c r="ED5" s="5"/>
+      <c r="EE5" s="5"/>
+      <c r="EF5" s="5"/>
+      <c r="EG5" s="5"/>
+      <c r="EH5" s="5"/>
+      <c r="EI5" s="5"/>
+      <c r="EJ5" s="5"/>
+      <c r="EK5" s="5"/>
+      <c r="EL5" s="5"/>
+      <c r="EM5" s="5"/>
+      <c r="EN5" s="5"/>
+      <c r="EO5" s="5"/>
+      <c r="EP5" s="5"/>
+      <c r="EQ5" s="5"/>
+      <c r="ER5" s="5"/>
+      <c r="ES5" s="5"/>
+      <c r="ET5" s="5"/>
+      <c r="EU5" s="5"/>
+      <c r="EV5" s="5"/>
+      <c r="EW5" s="5"/>
+      <c r="EX5" s="5"/>
+      <c r="EY5" s="5"/>
+      <c r="EZ5" s="5"/>
+      <c r="FA5" s="5"/>
+      <c r="FB5" s="5"/>
+      <c r="FC5" s="5"/>
+      <c r="FD5" s="5"/>
+      <c r="FE5" s="5"/>
+      <c r="FF5" s="5"/>
+      <c r="FG5" s="5"/>
+      <c r="FH5" s="5"/>
+      <c r="FI5" s="5"/>
+      <c r="FJ5" s="5"/>
+      <c r="FK5" s="5"/>
+      <c r="FL5" s="5"/>
+      <c r="FM5" s="5"/>
+      <c r="FN5" s="5"/>
+      <c r="FO5" s="5"/>
+      <c r="FP5" s="5"/>
+      <c r="FQ5" s="5"/>
+      <c r="FR5" s="5"/>
+      <c r="FS5" s="5"/>
+      <c r="FT5" s="5"/>
+      <c r="FU5" s="5"/>
+      <c r="FV5" s="5"/>
+      <c r="FW5" s="5"/>
+      <c r="FX5" s="5"/>
+      <c r="FY5" s="5"/>
+      <c r="FZ5" s="5"/>
+      <c r="GA5" s="5"/>
+      <c r="GB5" s="5"/>
+      <c r="GC5" s="5"/>
+      <c r="GD5" s="5"/>
+      <c r="GE5" s="5"/>
+      <c r="GF5" s="5"/>
+      <c r="GG5" s="5"/>
+      <c r="GH5" s="5"/>
+      <c r="GI5" s="5"/>
+      <c r="GJ5" s="5"/>
+      <c r="GK5" s="5"/>
+      <c r="GL5" s="5"/>
+      <c r="GM5" s="5"/>
+      <c r="GN5" s="5"/>
+      <c r="GO5" s="5"/>
+      <c r="GP5" s="5"/>
+      <c r="GQ5" s="5"/>
+      <c r="GR5" s="5"/>
+      <c r="GS5" s="5"/>
+      <c r="GT5" s="5"/>
+      <c r="GU5" s="5"/>
+      <c r="GV5" s="5"/>
+      <c r="GW5" s="5"/>
+      <c r="GX5" s="5"/>
+      <c r="GY5" s="5"/>
+      <c r="GZ5" s="5"/>
+      <c r="HA5" s="5"/>
+      <c r="HB5" s="5"/>
+      <c r="HC5" s="5"/>
+      <c r="HD5" s="5"/>
+      <c r="HE5" s="5"/>
+      <c r="HF5" s="5"/>
+      <c r="HG5" s="5"/>
+      <c r="HH5" s="5"/>
+      <c r="HI5" s="5"/>
+      <c r="HJ5" s="5"/>
+      <c r="HK5" s="5"/>
+      <c r="HL5" s="5"/>
+      <c r="HM5" s="5"/>
+      <c r="HN5" s="5"/>
+      <c r="HO5" s="5"/>
+      <c r="HP5" s="5"/>
+      <c r="HQ5" s="5"/>
+      <c r="HR5" s="5"/>
+      <c r="HS5" s="5"/>
+      <c r="HT5" s="5"/>
+      <c r="HU5" s="5"/>
+      <c r="HV5" s="5"/>
+      <c r="HW5" s="5"/>
+      <c r="HX5" s="5"/>
+      <c r="HY5" s="5"/>
+      <c r="HZ5" s="5"/>
+      <c r="IA5" s="5"/>
+      <c r="IB5" s="5"/>
+      <c r="IC5" s="5"/>
+      <c r="ID5" s="5"/>
+      <c r="IE5" s="5"/>
+      <c r="IF5" s="5"/>
+      <c r="IG5" s="5"/>
+      <c r="IH5" s="5"/>
+      <c r="II5" s="5"/>
+      <c r="IJ5" s="5"/>
+      <c r="IK5" s="5"/>
+      <c r="IL5" s="5"/>
+      <c r="IM5" s="5"/>
+      <c r="IN5" s="5"/>
+      <c r="IO5" s="5"/>
+      <c r="IP5" s="5"/>
+      <c r="IQ5" s="5"/>
+      <c r="IR5" s="5"/>
+      <c r="IS5" s="5"/>
+      <c r="IT5" s="5"/>
+      <c r="IU5" s="5"/>
+      <c r="IV5" s="5"/>
+      <c r="IW5" s="5"/>
+      <c r="IX5" s="5"/>
+      <c r="IY5" s="5"/>
+      <c r="IZ5" s="5"/>
+      <c r="JA5" s="5"/>
+      <c r="JB5" s="5"/>
+      <c r="JC5" s="5"/>
+      <c r="JD5" s="5"/>
+      <c r="JE5" s="5"/>
+      <c r="JF5" s="5"/>
+      <c r="JG5" s="5"/>
+      <c r="JH5" s="5"/>
+      <c r="JI5" s="5"/>
+      <c r="JJ5" s="5"/>
+      <c r="JK5" s="5"/>
+      <c r="JL5" s="5"/>
+      <c r="JM5" s="5"/>
+      <c r="JN5" s="5"/>
+      <c r="JO5" s="5"/>
+      <c r="JP5" s="5"/>
+      <c r="JQ5" s="5"/>
+      <c r="JR5" s="5"/>
+      <c r="JS5" s="5"/>
+      <c r="JT5" s="5"/>
+      <c r="JU5" s="5"/>
+      <c r="JV5" s="5"/>
+      <c r="JW5" s="5"/>
+      <c r="JX5" s="5"/>
+      <c r="JY5" s="5"/>
+      <c r="JZ5" s="5"/>
+      <c r="KA5" s="5"/>
+      <c r="KB5" s="5"/>
+      <c r="KC5" s="5"/>
+      <c r="KD5" s="5"/>
+      <c r="KE5" s="5"/>
+      <c r="KF5" s="5"/>
+      <c r="KG5" s="5"/>
+      <c r="KH5" s="5"/>
+      <c r="KI5" s="5"/>
+      <c r="KJ5" s="5"/>
+      <c r="KK5" s="5"/>
+      <c r="KL5" s="5"/>
+      <c r="KM5" s="5"/>
+      <c r="KN5" s="5"/>
+      <c r="KO5" s="5"/>
+      <c r="KP5" s="5"/>
+      <c r="KQ5" s="5"/>
+      <c r="KR5" s="5"/>
+      <c r="KS5" s="5"/>
+      <c r="KT5" s="5"/>
+      <c r="KU5" s="5"/>
+      <c r="KV5" s="5"/>
+      <c r="KW5" s="5"/>
+      <c r="KX5" s="5"/>
+      <c r="KY5" s="5"/>
+      <c r="KZ5" s="5"/>
+      <c r="LA5" s="5"/>
+      <c r="LB5" s="5"/>
+      <c r="LC5" s="5"/>
+      <c r="LD5" s="5"/>
+      <c r="LE5" s="5"/>
+      <c r="LF5" s="5"/>
+      <c r="LG5" s="5"/>
+      <c r="LH5" s="5"/>
+      <c r="LI5" s="5"/>
+      <c r="LJ5" s="5"/>
+      <c r="LK5" s="5"/>
+      <c r="LL5" s="5"/>
+      <c r="LM5" s="5"/>
+      <c r="LN5" s="5"/>
+      <c r="LO5" s="5"/>
+      <c r="LP5" s="5"/>
+      <c r="LQ5" s="5"/>
+      <c r="LR5" s="5"/>
+      <c r="LS5" s="5"/>
+      <c r="LT5" s="5"/>
+      <c r="LU5" s="5"/>
+      <c r="LV5" s="5"/>
+      <c r="LW5" s="5"/>
+      <c r="LX5" s="5"/>
+      <c r="LY5" s="5"/>
+      <c r="LZ5" s="5"/>
+      <c r="MA5" s="5"/>
+      <c r="MB5" s="5"/>
+      <c r="MC5" s="5"/>
+      <c r="MD5" s="5"/>
+      <c r="ME5" s="5"/>
+      <c r="MF5" s="5"/>
+      <c r="MG5" s="5"/>
+      <c r="MH5" s="5"/>
+      <c r="MI5" s="5"/>
+      <c r="MJ5" s="5"/>
+      <c r="MK5" s="5"/>
+      <c r="ML5" s="5"/>
+      <c r="MM5" s="5"/>
+      <c r="MN5" s="5"/>
+      <c r="MO5" s="5"/>
+      <c r="MP5" s="5"/>
+      <c r="MQ5" s="5"/>
+      <c r="MR5" s="5"/>
+      <c r="MS5" s="5"/>
+      <c r="MT5" s="5"/>
+      <c r="MU5" s="5"/>
+      <c r="MV5" s="5"/>
+      <c r="MW5" s="5"/>
+      <c r="MX5" s="5"/>
+      <c r="MY5" s="5"/>
+      <c r="MZ5" s="5"/>
+      <c r="NA5" s="5"/>
+      <c r="NB5" s="5"/>
+      <c r="NC5" s="5"/>
+      <c r="ND5" s="5"/>
+      <c r="NE5" s="5"/>
+      <c r="NF5" s="5"/>
+      <c r="NG5" s="5"/>
+      <c r="NH5" s="5"/>
+      <c r="NI5" s="5"/>
+      <c r="NJ5" s="5"/>
+      <c r="NK5" s="5"/>
+      <c r="NL5" s="5"/>
+      <c r="NM5" s="5"/>
+      <c r="NN5" s="5"/>
+      <c r="NO5" s="5"/>
+      <c r="NP5" s="5"/>
+      <c r="NQ5" s="5"/>
+      <c r="NR5" s="5"/>
+      <c r="NS5" s="5"/>
+      <c r="NT5" s="5"/>
+      <c r="NU5" s="5"/>
+      <c r="NV5" s="5"/>
+      <c r="NW5" s="5"/>
+      <c r="NX5" s="5"/>
+      <c r="NY5" s="5"/>
+      <c r="NZ5" s="5"/>
+      <c r="OA5" s="5"/>
+      <c r="OB5" s="5"/>
+      <c r="OC5" s="5"/>
+      <c r="OD5" s="5"/>
+      <c r="OE5" s="5"/>
+      <c r="OF5" s="5"/>
+      <c r="OG5" s="5"/>
+      <c r="OH5" s="5"/>
+      <c r="OI5" s="5"/>
+      <c r="OJ5" s="5"/>
+      <c r="OK5" s="5"/>
+      <c r="OL5" s="5"/>
+      <c r="OM5" s="5"/>
+      <c r="ON5" s="5"/>
+      <c r="OO5" s="5"/>
+      <c r="OP5" s="5"/>
+      <c r="OQ5" s="5"/>
+      <c r="OR5" s="5"/>
+      <c r="OS5" s="5"/>
+      <c r="OT5" s="5"/>
+      <c r="OU5" s="5"/>
+      <c r="OV5" s="5"/>
+      <c r="OW5" s="5"/>
+      <c r="OX5" s="5"/>
+      <c r="OY5" s="5"/>
+      <c r="OZ5" s="5"/>
+      <c r="PA5" s="5"/>
+      <c r="PB5" s="5"/>
+      <c r="PC5" s="5"/>
+      <c r="PD5" s="5"/>
+      <c r="PE5" s="5"/>
+      <c r="PF5" s="5"/>
+      <c r="PG5" s="5"/>
+      <c r="PH5" s="5"/>
+      <c r="PI5" s="5"/>
+      <c r="PJ5" s="5"/>
+      <c r="PK5" s="5"/>
+      <c r="PL5" s="5"/>
+      <c r="PM5" s="5"/>
+      <c r="PN5" s="5"/>
+      <c r="PO5" s="5"/>
+      <c r="PP5" s="5"/>
+      <c r="PQ5" s="5"/>
+      <c r="PR5" s="5"/>
+      <c r="PS5" s="5"/>
+      <c r="PT5" s="5"/>
+      <c r="PU5" s="5"/>
+      <c r="PV5" s="5"/>
+      <c r="PW5" s="5"/>
+      <c r="PX5" s="5"/>
+      <c r="PY5" s="5"/>
+      <c r="PZ5" s="5"/>
+      <c r="QA5" s="5"/>
+      <c r="QB5" s="5"/>
+      <c r="QC5" s="5"/>
+      <c r="QD5" s="5"/>
+      <c r="QE5" s="5"/>
+      <c r="QF5" s="5"/>
+      <c r="QG5" s="5"/>
+      <c r="QH5" s="5"/>
+      <c r="QI5" s="5"/>
+      <c r="QJ5" s="5"/>
+      <c r="QK5" s="5"/>
+      <c r="QL5" s="5"/>
+      <c r="QM5" s="5"/>
+      <c r="QN5" s="5"/>
+      <c r="QO5" s="5"/>
+      <c r="QP5" s="5"/>
+      <c r="QQ5" s="5"/>
     </row>
     <row r="6" spans="1:459" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1793,7 +1761,7 @@
       <c r="E6">
         <v>39.5</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H6">
@@ -1822,7 +1790,7 @@
       <c r="E7">
         <v>35.700000000000003</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H7">
@@ -1851,7 +1819,7 @@
       <c r="E8">
         <v>16.3</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H8">
@@ -1880,7 +1848,7 @@
       <c r="E9">
         <v>16.7</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="9" t="s">
         <v>32</v>
       </c>
       <c r="H9">
@@ -1909,7 +1877,7 @@
       <c r="E10">
         <v>23.4</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="10" t="s">
         <v>33</v>
       </c>
       <c r="H10">
@@ -1938,7 +1906,7 @@
       <c r="E11">
         <v>18.3</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="H11">
@@ -1967,7 +1935,7 @@
       <c r="E12">
         <v>35.200000000000003</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="12" t="s">
         <v>38</v>
       </c>
       <c r="H12">
@@ -1981,18 +1949,18 @@
       </c>
     </row>
     <row r="14" spans="1:459" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="G14" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:459" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2036,7 +2004,7 @@
       <c r="E16">
         <v>26.5</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="25" t="s">
         <v>52</v>
       </c>
       <c r="H16">
@@ -2065,7 +2033,7 @@
       <c r="E17">
         <v>30.1</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="13" t="s">
         <v>41</v>
       </c>
       <c r="H17">
@@ -2094,7 +2062,7 @@
       <c r="E18">
         <v>19.600000000000001</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="H18">
@@ -2123,7 +2091,7 @@
       <c r="E19">
         <v>7.7</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H19">
@@ -2152,7 +2120,7 @@
       <c r="E20">
         <v>13.6</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="15" t="s">
         <v>43</v>
       </c>
       <c r="H20">
@@ -2181,7 +2149,7 @@
       <c r="E21">
         <v>9.5</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="17" t="s">
         <v>45</v>
       </c>
       <c r="H21">
@@ -2210,7 +2178,7 @@
       <c r="E22">
         <v>8.6</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="18" t="s">
         <v>46</v>
       </c>
       <c r="H22">
@@ -2239,7 +2207,7 @@
       <c r="E23">
         <v>11.3</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="24" t="s">
         <v>51</v>
       </c>
       <c r="H23">
@@ -2268,7 +2236,7 @@
       <c r="E24">
         <v>18.7</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="21" t="s">
         <v>49</v>
       </c>
       <c r="H24">
@@ -2297,7 +2265,7 @@
       <c r="E25">
         <v>12.8</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="22" t="s">
         <v>50</v>
       </c>
       <c r="H25">
@@ -2326,7 +2294,7 @@
       <c r="E26">
         <v>15</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="23" t="s">
         <v>46</v>
       </c>
       <c r="H26">
@@ -2355,7 +2323,7 @@
       <c r="E27">
         <v>15.5</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="19" t="s">
         <v>47</v>
       </c>
       <c r="H27">
@@ -2384,7 +2352,7 @@
       <c r="E28">
         <v>11.7</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="20" t="s">
         <v>48</v>
       </c>
       <c r="H28">
@@ -2395,281 +2363,6 @@
       </c>
       <c r="J28">
         <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="23">
-        <v>16.3</v>
-      </c>
-      <c r="C32" s="26">
-        <f>B32*(10^6)/3600</f>
-        <v>4527.7777777777774</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="23">
-        <v>9.5</v>
-      </c>
-      <c r="C33" s="26">
-        <f t="shared" ref="C33:C53" si="0">B33*(10^6)/3600</f>
-        <v>2638.8888888888887</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="23">
-        <v>16.7</v>
-      </c>
-      <c r="C34" s="26">
-        <f t="shared" si="0"/>
-        <v>4638.8888888888887</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="23">
-        <v>18.2</v>
-      </c>
-      <c r="C35" s="26">
-        <f t="shared" si="0"/>
-        <v>5055.5555555555557</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="23">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="C36" s="26">
-        <f t="shared" si="0"/>
-        <v>5444.4444444444443</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" s="23">
-        <v>23.4</v>
-      </c>
-      <c r="C37" s="26">
-        <f t="shared" si="0"/>
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="23">
-        <v>18.3</v>
-      </c>
-      <c r="C38" s="26">
-        <f t="shared" si="0"/>
-        <v>5083.333333333333</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="23">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="C39" s="26">
-        <f t="shared" si="0"/>
-        <v>9916.6666666666661</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="23">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="C40" s="26">
-        <f t="shared" si="0"/>
-        <v>9777.7777777777774</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="23">
-        <v>30.1</v>
-      </c>
-      <c r="C41" s="26">
-        <f t="shared" si="0"/>
-        <v>8361.1111111111113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="23">
-        <v>39.5</v>
-      </c>
-      <c r="C42" s="26">
-        <f t="shared" si="0"/>
-        <v>10972.222222222223</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" s="23">
-        <v>15</v>
-      </c>
-      <c r="C43" s="26">
-        <f t="shared" si="0"/>
-        <v>4166.666666666667</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="23">
-        <v>15.5</v>
-      </c>
-      <c r="C44" s="26">
-        <f t="shared" si="0"/>
-        <v>4305.5555555555557</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="23">
-        <v>11.3</v>
-      </c>
-      <c r="C45" s="26">
-        <f t="shared" si="0"/>
-        <v>3138.8888888888887</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="23">
-        <v>18.7</v>
-      </c>
-      <c r="C46" s="26">
-        <f t="shared" si="0"/>
-        <v>5194.4444444444443</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="23">
-        <v>11.7</v>
-      </c>
-      <c r="C47" s="26">
-        <f t="shared" si="0"/>
-        <v>3250</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="23">
-        <v>9.5</v>
-      </c>
-      <c r="C48" s="26">
-        <f t="shared" si="0"/>
-        <v>2638.8888888888887</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="23">
-        <v>7.7</v>
-      </c>
-      <c r="C49" s="26">
-        <f t="shared" si="0"/>
-        <v>2138.8888888888887</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="23">
-        <v>13.6</v>
-      </c>
-      <c r="C50" s="26">
-        <f t="shared" si="0"/>
-        <v>3777.7777777777778</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="23">
-        <v>26.5</v>
-      </c>
-      <c r="C51" s="26">
-        <f t="shared" si="0"/>
-        <v>7361.1111111111113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B52" s="23">
-        <v>12.8</v>
-      </c>
-      <c r="C52" s="26">
-        <f t="shared" si="0"/>
-        <v>3555.5555555555557</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="23">
-        <v>8.6</v>
-      </c>
-      <c r="C53" s="26">
-        <f t="shared" si="0"/>
-        <v>2388.8888888888887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>